<commit_message>
export calendar functions to Excel (52/1114)
</commit_message>
<xml_diff>
--- a/UnitTests/Tests/Calendars.xlsx
+++ b/UnitTests/Tests/Calendars.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Function</t>
   </si>
@@ -498,16 +498,16 @@
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D3" s="4" t="e">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="str">
         <f>IF(B3=C3,"PASS","FAIL")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E3" t="e">
-        <f ca="1">_xll.qlCalendarName("target")</f>
-        <v>#NAME?</v>
+        <v>PASS</v>
+      </c>
+      <c r="E3" t="str">
+        <f>_xll.qlCalendarName("target")</f>
+        <v>TARGET</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -517,16 +517,16 @@
       <c r="B4" t="b">
         <v>0</v>
       </c>
-      <c r="C4" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D4" s="4" t="e">
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="str">
         <f t="shared" ref="D4:D13" si="0">IF(B4=C4,"PASS","FAIL")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E4" t="e">
-        <f ca="1">_xll.qlCalendarIsBusinessDay("target",25569)</f>
-        <v>#NAME?</v>
+        <v>PASS</v>
+      </c>
+      <c r="E4" t="b">
+        <f>_xll.qlCalendarIsBusinessDay("target",25569)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -536,16 +536,16 @@
       <c r="B5" t="b">
         <v>1</v>
       </c>
-      <c r="C5" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D5" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E5" t="e">
-        <f ca="1">_xll.qlCalendarIsHoliday("target",25569)</f>
-        <v>#NAME?</v>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E5" t="b">
+        <f>_xll.qlCalendarIsHoliday("target",25569)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -555,16 +555,16 @@
       <c r="B6" t="b">
         <v>0</v>
       </c>
-      <c r="C6" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D6" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E6" t="e">
-        <f ca="1">_xll.qlCalendarIsEndOfMonth("target",25569)</f>
-        <v>#NAME?</v>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E6" t="b">
+        <f>_xll.qlCalendarIsEndOfMonth("target",25569)</f>
+        <v>0</v>
       </c>
       <c r="F6" s="5"/>
     </row>
@@ -575,16 +575,16 @@
       <c r="B7">
         <v>25598</v>
       </c>
-      <c r="C7" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D7" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E7" t="e">
-        <f ca="1">_xll.qlCalendarEndOfMonth("target",25569)</f>
-        <v>#NAME?</v>
+      <c r="C7">
+        <v>25598</v>
+      </c>
+      <c r="D7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E7">
+        <f>_xll.qlCalendarEndOfMonth("target",25569)</f>
+        <v>25598</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -594,16 +594,16 @@
       <c r="B8" t="b">
         <v>1</v>
       </c>
-      <c r="C8" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D8" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E8" t="e">
-        <f ca="1">_xll.qlCalendarAddHoliday("london",25569)</f>
-        <v>#NAME?</v>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E8" t="b">
+        <f>_xll.qlCalendarAddHoliday("london",25569)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -613,16 +613,16 @@
       <c r="B9" t="b">
         <v>1</v>
       </c>
-      <c r="C9" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D9" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E9" t="e">
-        <f ca="1">_xll.qlCalendarRemoveHoliday("japan",25569)</f>
-        <v>#NAME?</v>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E9" t="b">
+        <f>_xll.qlCalendarRemoveHoliday("japan",25569)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -632,16 +632,16 @@
       <c r="B10">
         <v>42005</v>
       </c>
-      <c r="C10" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D10" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E10" t="e">
-        <f ca="1">_xll.qlCalendarHolidayList("target",42005,42369)</f>
-        <v>#NAME?</v>
+      <c r="C10">
+        <v>42005</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E10">
+        <f>_xll.qlCalendarHolidayList("target",42005,42369)</f>
+        <v>42005</v>
       </c>
       <c r="G10" s="5">
         <v>42005</v>
@@ -654,16 +654,16 @@
       <c r="B11">
         <v>25570</v>
       </c>
-      <c r="C11" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D11" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E11" t="e">
-        <f ca="1">_xll.qlCalendarAdjust("target",25569)</f>
-        <v>#NAME?</v>
+      <c r="C11">
+        <v>25570</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E11">
+        <f>_xll.qlCalendarAdjust("target",25569)</f>
+        <v>25570</v>
       </c>
       <c r="G11" s="5">
         <v>42369</v>
@@ -676,16 +676,16 @@
       <c r="B12">
         <v>25570</v>
       </c>
-      <c r="C12" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D12" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E12" t="e">
-        <f ca="1">_xll.qlCalendarAdvance("target",25569,"1d")</f>
-        <v>#NAME?</v>
+      <c r="C12">
+        <v>25570</v>
+      </c>
+      <c r="D12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E12">
+        <f>_xll.qlCalendarAdvance("target",25569,"1d")</f>
+        <v>25570</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -695,16 +695,16 @@
       <c r="B13">
         <v>255</v>
       </c>
-      <c r="C13" t="e">
-        <v>#NAME?</v>
-      </c>
-      <c r="D13" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E13" t="e">
-        <f ca="1">_xll.qlCalendarBusinessDaysBetween("target",42005,42369)</f>
-        <v>#NAME?</v>
+      <c r="C13">
+        <v>255</v>
+      </c>
+      <c r="D13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>PASS</v>
+      </c>
+      <c r="E13">
+        <f>_xll.qlCalendarBusinessDaysBetween("target",42005,42369)</f>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>